<commit_message>
NP comparisons within seasons
</commit_message>
<xml_diff>
--- a/results/comparison-letters-templates/np_comparison_letters_within_season.xlsx
+++ b/results/comparison-letters-templates/np_comparison_letters_within_season.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\CU\Data\toronto-lmb-np-accel\results\comparison-letters-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18A8DDB-BDC2-451E-B68F-C4EB47CC7EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BEB184-A63A-4883-A204-6F3EB4602E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9A924BF9-6E79-484A-812B-34246742B6BC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="34">
   <si>
     <t xml:space="preserve">Habitat Type </t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>l</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>****</t>
   </si>
 </sst>
 </file>
@@ -188,14 +200,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -514,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{958CDEBC-A36B-40FB-93F3-09AA5706FC28}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,7 +591,7 @@
       <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -604,13 +614,13 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E5" t="s">
@@ -639,7 +649,7 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
@@ -653,16 +663,22 @@
       </c>
       <c r="F6" t="s">
         <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
@@ -671,7 +687,7 @@
       <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -679,7 +695,7 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
@@ -705,7 +721,7 @@
       <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -744,7 +760,7 @@
       <c r="F13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H13" s="3" t="s">
@@ -810,6 +826,9 @@
       </c>
       <c r="F15" t="s">
         <v>19</v>
+      </c>
+      <c r="I15" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -891,7 +910,7 @@
       <c r="F22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H22" s="3" t="s">
@@ -957,6 +976,12 @@
       </c>
       <c r="E24" t="s">
         <v>21</v>
+      </c>
+      <c r="I24" t="s">
+        <v>31</v>
+      </c>
+      <c r="K24" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -1048,7 +1073,7 @@
       <c r="F33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H33" s="3" t="s">
@@ -1093,6 +1118,12 @@
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>3</v>
+      </c>
+      <c r="I35" t="s">
+        <v>32</v>
+      </c>
+      <c r="K35" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>